<commit_message>
Fix: Fixed try_print_anvisa_register method and added exception handling in Google search
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Item</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>Torrent</t>
-  </si>
-  <si>
-    <t>Sucesso</t>
   </si>
   <si>
     <t>Falha</t>
@@ -484,7 +481,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -526,7 +523,7 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: fixed error when trying to rename files with an existing name
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>Item</t>
   </si>
@@ -28,73 +28,16 @@
     <t>Registro</t>
   </si>
   <si>
-    <t>HEPARINA SODICA SUBCUT 5000UI</t>
-  </si>
-  <si>
-    <t>PROMETAZINA PROFERGAN</t>
-  </si>
-  <si>
-    <t>HALOPERIDOL 5MG</t>
-  </si>
-  <si>
-    <t>CLORPROMAZINA 40MG/ML SOL ORAL</t>
-  </si>
-  <si>
-    <t>HALOPERIDOL 2MG/ML SOL ORAL</t>
-  </si>
-  <si>
-    <t>CLORPROMAZINA 25MG</t>
-  </si>
-  <si>
-    <t>FOSFATO DE CODEÍNA CODEIN</t>
-  </si>
-  <si>
-    <t>CLORIDRATO DE IMIPRAMINA IMIPRA</t>
-  </si>
-  <si>
-    <t>RISPERIDONA RISPERIDONA</t>
-  </si>
-  <si>
-    <t>LEVOMEPROMAZINA 4% GOTAS</t>
-  </si>
-  <si>
-    <t>LIDOCAÍNA XYLESTESIN</t>
-  </si>
-  <si>
-    <t>NITRATO DE CERIO +SULFADIAZINA</t>
-  </si>
-  <si>
-    <t>COLAGENASE KOLLAGENASE</t>
-  </si>
-  <si>
-    <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
-  </si>
-  <si>
-    <t>LABORATÓRIO TEUTO BRASILEIRO S/A</t>
-  </si>
-  <si>
-    <t>CELLERA FARMACÊUTICA S.A.</t>
-  </si>
-  <si>
-    <t>SANOFI MEDLEY FARMACÊUTICA LTDA</t>
-  </si>
-  <si>
-    <t>VITAMEDIC INDUSTRIA FARMACEUTICA LTDA</t>
-  </si>
-  <si>
-    <t>102980371</t>
-  </si>
-  <si>
-    <t>183260385</t>
-  </si>
-  <si>
-    <t>183260316</t>
-  </si>
-  <si>
-    <t>102980560</t>
-  </si>
-  <si>
-    <t>102980431</t>
+    <t>CLORETO DE SÓDIO JP FISIOLÓGICO</t>
+  </si>
+  <si>
+    <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
+  </si>
+  <si>
+    <t>JP INDUSTRIA FARMACEUTICA S/A</t>
+  </si>
+  <si>
+    <t>104910020</t>
   </si>
 </sst>
 </file>
@@ -452,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -474,198 +417,58 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>104910070</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>103700321</v>
+        <v>104910070</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
       <c r="D4">
-        <v>112360011</v>
+        <v>104910070</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6">
-        <v>112360011</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8">
-        <v>102980199</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9">
-        <v>102980023</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10">
-        <v>103920197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11">
-        <v>103920197</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13">
-        <v>102980357</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added PDF feedback functionality
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>Item</t>
   </si>
@@ -28,16 +28,124 @@
     <t>Registro</t>
   </si>
   <si>
-    <t>CLORETO DE SÓDIO JP FISIOLÓGICO</t>
-  </si>
-  <si>
-    <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
-  </si>
-  <si>
-    <t>JP INDUSTRIA FARMACEUTICA S/A</t>
-  </si>
-  <si>
-    <t>104910020</t>
+    <t>PDF</t>
+  </si>
+  <si>
+    <t>Tempo Decorrido</t>
+  </si>
+  <si>
+    <t>HEPARINA SODICA SUBCUT 5000UI</t>
+  </si>
+  <si>
+    <t>PROMETAZINA PROFERGAN</t>
+  </si>
+  <si>
+    <t>HALOPERIDOL 5MG</t>
+  </si>
+  <si>
+    <t>CLORPROMAZINA 40MG/ML SOL ORAL</t>
+  </si>
+  <si>
+    <t>HALOPERIDOL 2MG/ML SOL ORAL</t>
+  </si>
+  <si>
+    <t>CLORPROMAZINA 25MG</t>
+  </si>
+  <si>
+    <t>FOSFATO DE CODEÍNA CODEIN</t>
+  </si>
+  <si>
+    <t>CLORIDRATO DE IMIPRAMINA IMIPRA</t>
+  </si>
+  <si>
+    <t>RISPERIDONA RISPERIDONA</t>
+  </si>
+  <si>
+    <t>LEVOMEPROMAZINA 4% GOTAS</t>
+  </si>
+  <si>
+    <t>LIDOCAÍNA XYLESTESIN</t>
+  </si>
+  <si>
+    <t>NITRATO DE CERIO +SULFADIAZINA</t>
+  </si>
+  <si>
+    <t>COLAGENASE KOLLAGENASE</t>
+  </si>
+  <si>
+    <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
+  </si>
+  <si>
+    <t>LABORATÓRIO TEUTO BRASILEIRO S/A</t>
+  </si>
+  <si>
+    <t>CELLERA FARMACÊUTICA S.A.</t>
+  </si>
+  <si>
+    <t>SANOFI MEDLEY FARMACÊUTICA LTDA</t>
+  </si>
+  <si>
+    <t>VITAMEDIC INDUSTRIA FARMACEUTICA LTDA</t>
+  </si>
+  <si>
+    <t>102980371</t>
+  </si>
+  <si>
+    <t>183260385</t>
+  </si>
+  <si>
+    <t>183260316</t>
+  </si>
+  <si>
+    <t>102980560</t>
+  </si>
+  <si>
+    <t>102980431</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 29.90 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 13.45 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 14.38 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 29.00 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 13.53 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 29.53 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 13.26 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 13.69 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 12.81 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 13.92 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 28.47 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 13.30 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 30.09 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 30.70 seconds</t>
   </si>
 </sst>
 </file>
@@ -395,13 +503,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,61 +522,291 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>103700321</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>112360011</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
         <v>6</v>
       </c>
-      <c r="D2">
-        <v>104910070</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>104910070</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>112360011</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>104910070</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>102980199</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>102980023</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <v>103920197</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11">
+        <v>103920197</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>102980357</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added expired register filter to SMERP searches
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -106,46 +106,46 @@
     <t>OK</t>
   </si>
   <si>
+    <t>0 hours, 0 minutes, and 32.78 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 13.49 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 13.70 seconds</t>
+  </si>
+  <si>
     <t>0 hours, 0 minutes, and 29.90 seconds</t>
   </si>
   <si>
-    <t>0 hours, 0 minutes, and 13.45 seconds</t>
-  </si>
-  <si>
-    <t>0 hours, 0 minutes, and 14.38 seconds</t>
-  </si>
-  <si>
-    <t>0 hours, 0 minutes, and 29.00 seconds</t>
-  </si>
-  <si>
-    <t>0 hours, 0 minutes, and 13.53 seconds</t>
-  </si>
-  <si>
-    <t>0 hours, 0 minutes, and 29.53 seconds</t>
-  </si>
-  <si>
-    <t>0 hours, 0 minutes, and 13.26 seconds</t>
-  </si>
-  <si>
-    <t>0 hours, 0 minutes, and 13.69 seconds</t>
-  </si>
-  <si>
-    <t>0 hours, 0 minutes, and 12.81 seconds</t>
-  </si>
-  <si>
-    <t>0 hours, 0 minutes, and 13.92 seconds</t>
-  </si>
-  <si>
-    <t>0 hours, 0 minutes, and 28.47 seconds</t>
-  </si>
-  <si>
-    <t>0 hours, 0 minutes, and 13.30 seconds</t>
-  </si>
-  <si>
-    <t>0 hours, 0 minutes, and 30.09 seconds</t>
-  </si>
-  <si>
-    <t>0 hours, 0 minutes, and 30.70 seconds</t>
+    <t>0 hours, 0 minutes, and 14.35 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 30.49 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 12.29 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 14.68 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 12.98 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 13.38 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 28.75 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 13.66 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 31.00 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 34.66 seconds</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
feat: Implementation of PDF storage and efficiency enhancement in retrieving PDF registers
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Item</t>
   </si>
@@ -46,13 +46,19 @@
     <t>104910020</t>
   </si>
   <si>
-    <t>Pendente</t>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 15.39 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 0.11 seconds</t>
   </si>
   <si>
     <t>0 hours, 0 minutes, and 0.10 seconds</t>
   </si>
   <si>
-    <t>0 hours, 0 minutes, and 18.70 seconds</t>
+    <t>0 hours, 0 minutes, and 31.16 seconds</t>
   </si>
 </sst>
 </file>
@@ -473,7 +479,7 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -493,7 +499,7 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -513,7 +519,7 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: Optimized description processing
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -34,7 +34,7 @@
     <t>Tempo Decorrido</t>
   </si>
   <si>
-    <t>CLORETO DE SÓDIO JP FISIOLÓGICO</t>
+    <t>GLICOSE;CLORETO DE SÓDIO</t>
   </si>
   <si>
     <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
@@ -49,7 +49,7 @@
     <t>OK</t>
   </si>
   <si>
-    <t>0 hours, 0 minutes, and 15.39 seconds</t>
+    <t>0 hours, 0 minutes, and 0.16 seconds</t>
   </si>
   <si>
     <t>0 hours, 0 minutes, and 0.11 seconds</t>
@@ -58,7 +58,7 @@
     <t>0 hours, 0 minutes, and 0.10 seconds</t>
   </si>
   <si>
-    <t>0 hours, 0 minutes, and 31.16 seconds</t>
+    <t>0 hours, 0 minutes, and 22.78 seconds</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
feat: implemented the creation of a data map of laboratory registers
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -49,16 +49,16 @@
     <t>OK</t>
   </si>
   <si>
-    <t>0 hours, 0 minutes, and 0.16 seconds</t>
-  </si>
-  <si>
-    <t>0 hours, 0 minutes, and 0.11 seconds</t>
-  </si>
-  <si>
-    <t>0 hours, 0 minutes, and 0.10 seconds</t>
-  </si>
-  <si>
-    <t>0 hours, 0 minutes, and 22.78 seconds</t>
+    <t>0 hours, 3 minutes, and 44.88 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 5.64 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 0.57 seconds</t>
+  </si>
+  <si>
+    <t>0 hours, 0 minutes, and 21.12 seconds</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
refactor: split Test class responsibilities into separate functions
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Item</t>
   </si>
@@ -34,16 +34,28 @@
     <t>PDF</t>
   </si>
   <si>
-    <t>aciclovir</t>
-  </si>
-  <si>
-    <t>250mg/ml</t>
-  </si>
-  <si>
-    <t>cimed</t>
-  </si>
-  <si>
-    <t>143810181</t>
+    <t>CLORETO DE SÓDIO;GLICOSE</t>
+  </si>
+  <si>
+    <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
+  </si>
+  <si>
+    <t>1000ml</t>
+  </si>
+  <si>
+    <t>250ml</t>
+  </si>
+  <si>
+    <t>500ml</t>
+  </si>
+  <si>
+    <t>JP INDUSTRIA FARMACEUTICA S/A</t>
+  </si>
+  <si>
+    <t>104910019</t>
+  </si>
+  <si>
+    <t>104910020</t>
   </si>
   <si>
     <t>Pendente</t>
@@ -404,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -432,22 +444,82 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added JSON file based database checking
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="297">
   <si>
     <t>Item</t>
   </si>
@@ -91,6 +91,9 @@
     <t>CARBAMAZEPINA</t>
   </si>
   <si>
+    <t>CARBONATO DE CÁLCIO</t>
+  </si>
+  <si>
     <t>CARBONATO DE LÍTIO</t>
   </si>
   <si>
@@ -202,6 +205,9 @@
     <t>GLICLAZIDA</t>
   </si>
   <si>
+    <t>GLICOSE</t>
+  </si>
+  <si>
     <t>HALOPERIDOL</t>
   </si>
   <si>
@@ -253,6 +259,9 @@
     <t>MICONAZOL</t>
   </si>
   <si>
+    <t>NITRATO DE MICONAZOL</t>
+  </si>
+  <si>
     <t>NITROFURANTOÍNA</t>
   </si>
   <si>
@@ -289,6 +298,12 @@
     <t>SULFATO DE SALBUTAMOL</t>
   </si>
   <si>
+    <t>SULFATO FERROSO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FITA PARA TESTES DE GLICEMIA COMPATIVEL PARA O APARELHO ACCU-CHEK ACTIVE </t>
+  </si>
+  <si>
     <t>VARFARINA SÓDICA</t>
   </si>
   <si>
@@ -421,6 +436,9 @@
     <t>60mg</t>
   </si>
   <si>
+    <t>Concentração não encontrada</t>
+  </si>
+  <si>
     <t>10mg</t>
   </si>
   <si>
@@ -466,6 +484,9 @@
     <t>100mcg</t>
   </si>
   <si>
+    <t>125 mg/ml</t>
+  </si>
+  <si>
     <t>LABORATÓRIOS OSÓRIO DE MORAES LTDA</t>
   </si>
   <si>
@@ -508,6 +529,9 @@
     <t>GERMED FARMACEUTICA LTDA</t>
   </si>
   <si>
+    <t>Nutivit/Imec</t>
+  </si>
+  <si>
     <t>NOVA QUIMICA FARMACÊUTICA S/A</t>
   </si>
   <si>
@@ -538,6 +562,9 @@
     <t>ACHÉ LABORATÓRIOS FARMACÊUTICOS S.A</t>
   </si>
   <si>
+    <t>On Call Plus</t>
+  </si>
+  <si>
     <t>LEGRAND PHARMA INDÚSTRIA FARMACÊUTICA LTDA</t>
   </si>
   <si>
@@ -562,6 +589,9 @@
     <t>PHARMASCIENCE INDUSTRIA FARMACEUTICA S.A</t>
   </si>
   <si>
+    <t>Arte Nativa</t>
+  </si>
+  <si>
     <t>UNIÃO QUÍMICA FARMACÊUTICA NACIONAL S/A</t>
   </si>
   <si>
@@ -620,6 +650,9 @@
   </si>
   <si>
     <t>105830847</t>
+  </si>
+  <si>
+    <t>Não encontrado</t>
   </si>
   <si>
     <t>109740309</t>
@@ -1229,7 +1262,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F122"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1263,16 +1296,16 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="E2" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="F2" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1283,16 +1316,16 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="E3" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="F3" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1303,16 +1336,16 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="E4" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="F4" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1323,16 +1356,16 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="E5" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="F5" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1343,16 +1376,16 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E6" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="F6" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1363,16 +1396,16 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D7" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E7" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="F7" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1383,16 +1416,16 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D8" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="E8" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="F8" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1403,16 +1436,16 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D9" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="E9" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="F9" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1423,16 +1456,16 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D10" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="E10" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="F10" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1443,16 +1476,16 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="E11" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="F11" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1463,16 +1496,16 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="E12" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="F12" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1483,16 +1516,16 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D13" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="E13" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="F13" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1503,16 +1536,16 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D14" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="E14" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="F14" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1523,16 +1556,16 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="D15" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="E15" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="F15" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1543,16 +1576,16 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D16" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="E16" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="F16" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1563,16 +1596,16 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D17" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="E17" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="F17" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1583,16 +1616,16 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D18" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="E18" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="F18" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1603,16 +1636,16 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D19" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E19" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="F19" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1623,16 +1656,16 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D20" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="E20" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="F20" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1643,16 +1676,16 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D21" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="E21" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="F21" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1663,16 +1696,16 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D22" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="E22" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="F22" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1683,16 +1716,16 @@
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D23" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="E23" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="F23" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1703,16 +1736,16 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D24" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="E24" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="F24" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1723,1956 +1756,2056 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D25" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="E25" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="F25" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D26" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
       <c r="E26" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="F26" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D27" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E27" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="F27" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="D28" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E28" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="F28" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="D29" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E29" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="F29" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
         <v>108</v>
       </c>
       <c r="D30" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E30" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="F30" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
         <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="D31" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E31" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F31" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="D32" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="E32" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="F32" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D33" t="s">
         <v>165</v>
       </c>
       <c r="E33" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="F33" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="D34" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="E34" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="F34" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
         <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D35" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="E35" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="F35" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
         <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D36" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E36" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="F36" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D37" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="E37" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="F37" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C38" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D38" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="E38" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="F38" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
         <v>32</v>
       </c>
       <c r="C39" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D39" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="E39" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="F39" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
         <v>33</v>
       </c>
       <c r="C40" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D40" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E40" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="F40" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
         <v>34</v>
       </c>
       <c r="C41" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D41" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="E41" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="F41" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
         <v>35</v>
       </c>
       <c r="C42" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D42" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E42" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="F42" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
         <v>36</v>
       </c>
       <c r="C43" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D43" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E43" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="F43" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
         <v>37</v>
       </c>
       <c r="C44" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D44" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E44" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="F44" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C45" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D45" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="E45" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="F45" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C46" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D46" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="E46" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="F46" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s">
         <v>38</v>
       </c>
       <c r="C47" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D47" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="E47" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="F47" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
         <v>39</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="D48" t="s">
         <v>169</v>
       </c>
       <c r="E48" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="F48" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s">
         <v>40</v>
       </c>
       <c r="C49" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D49" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="E49" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="F49" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50" t="s">
         <v>41</v>
       </c>
       <c r="C50" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D50" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="E50" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="F50" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B51" t="s">
         <v>42</v>
       </c>
       <c r="C51" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D51" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E51" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="F51" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52" t="s">
         <v>43</v>
       </c>
       <c r="C52" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D52" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="E52" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="F52" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C53" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D53" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="E53" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="F53" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B54" t="s">
         <v>44</v>
       </c>
       <c r="C54" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="D54" t="s">
         <v>160</v>
       </c>
       <c r="E54" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="F54" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D55" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E55" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="F55" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B56" t="s">
         <v>45</v>
       </c>
       <c r="C56" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="D56" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="E56" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="F56" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B57" t="s">
         <v>46</v>
       </c>
       <c r="C57" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="D57" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="E57" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="F57" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
         <v>47</v>
       </c>
       <c r="C58" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D58" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E58" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="F58" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="D59" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E59" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="F59" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B60" t="s">
         <v>48</v>
       </c>
       <c r="C60" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D60" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="E60" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="F60" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B61" t="s">
         <v>49</v>
       </c>
       <c r="C61" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D61" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E61" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="F61" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
         <v>50</v>
       </c>
       <c r="C62" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="D62" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E62" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="F62" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C63" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="D63" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="E63" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="F63" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C64" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="D64" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E64" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="F64" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B65" t="s">
         <v>51</v>
       </c>
       <c r="C65" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="D65" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="E65" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="F65" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B66" t="s">
         <v>52</v>
       </c>
       <c r="C66" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="D66" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E66" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="F66" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B67" t="s">
         <v>53</v>
       </c>
       <c r="C67" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D67" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="E67" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="F67" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B68" t="s">
         <v>54</v>
       </c>
       <c r="C68" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="D68" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="E68" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="F68" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B69" t="s">
         <v>55</v>
       </c>
       <c r="C69" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="D69" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="E69" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="F69" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B70" t="s">
         <v>56</v>
       </c>
       <c r="C70" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="D70" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
       <c r="E70" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="F70" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B71" t="s">
         <v>57</v>
       </c>
       <c r="C71" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D71" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E71" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="F71" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B72" t="s">
         <v>58</v>
       </c>
       <c r="C72" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D72" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="E72" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="F72" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B73" t="s">
         <v>59</v>
       </c>
       <c r="C73" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D73" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="E73" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="F73" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B74" t="s">
         <v>60</v>
       </c>
       <c r="C74" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="D74" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="E74" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="F74" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B75" t="s">
         <v>61</v>
       </c>
       <c r="C75" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="D75" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="E75" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="F75" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B76" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C76" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D76" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E76" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="F76" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B77" t="s">
         <v>62</v>
       </c>
       <c r="C77" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="D77" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="E77" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="F77" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B78" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C78" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="D78" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
       <c r="E78" t="s">
-        <v>243</v>
+        <v>212</v>
       </c>
       <c r="F78" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B79" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C79" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="D79" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="E79" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="F79" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B80" t="s">
         <v>64</v>
       </c>
       <c r="C80" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="D80" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E80" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="F80" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B81" t="s">
         <v>65</v>
       </c>
       <c r="C81" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="D81" t="s">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="E81" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="F81" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B82" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C82" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D82" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="E82" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="F82" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B83" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C83" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="D83" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E83" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="F83" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B84" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C84" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="D84" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E84" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="F84" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B85" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C85" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="D85" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="E85" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="F85" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B86" t="s">
         <v>68</v>
       </c>
       <c r="C86" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D86" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="E86" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="F86" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B87" t="s">
         <v>69</v>
       </c>
       <c r="C87" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="D87" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="E87" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="F87" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B88" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C88" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D88" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E88" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="F88" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B89" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C89" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D89" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="E89" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="F89" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B90" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C90" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="D90" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="E90" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="F90" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B91" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C91" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="D91" t="s">
-        <v>153</v>
+        <v>184</v>
       </c>
       <c r="E91" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="F91" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B92" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C92" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="D92" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="E92" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="F92" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B93" t="s">
         <v>72</v>
       </c>
       <c r="C93" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="D93" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E93" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="F93" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B94" t="s">
         <v>73</v>
       </c>
       <c r="C94" t="s">
-        <v>142</v>
+        <v>111</v>
       </c>
       <c r="D94" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="E94" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="F94" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B95" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C95" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="D95" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="E95" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="F95" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B96" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C96" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D96" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="E96" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="F96" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B97" t="s">
         <v>75</v>
       </c>
       <c r="C97" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D97" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E97" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="F97" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B98" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C98" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="D98" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="E98" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="F98" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B99" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C99" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="D99" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="E99" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="F99" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B100" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C100" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="D100" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="E100" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="F100" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B101" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C101" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D101" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E101" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="F101" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B102" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C102" t="s">
-        <v>99</v>
+        <v>150</v>
       </c>
       <c r="D102" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="E102" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="F102" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B103" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C103" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="D103" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="E103" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="F103" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B104" t="s">
         <v>79</v>
       </c>
       <c r="C104" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="D104" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="E104" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="F104" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B105" t="s">
         <v>80</v>
       </c>
       <c r="C105" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="D105" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="E105" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="F105" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B106" t="s">
         <v>81</v>
       </c>
       <c r="C106" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="D106" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E106" t="s">
-        <v>268</v>
+        <v>212</v>
       </c>
       <c r="F106" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B107" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C107" t="s">
-        <v>144</v>
+        <v>99</v>
       </c>
       <c r="D107" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E107" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="F107" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B108" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C108" t="s">
-        <v>145</v>
+        <v>107</v>
       </c>
       <c r="D108" t="s">
-        <v>153</v>
+        <v>186</v>
       </c>
       <c r="E108" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="F108" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B109" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C109" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="D109" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
       <c r="E109" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="F109" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B110" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C110" t="s">
-        <v>97</v>
+        <v>150</v>
       </c>
       <c r="D110" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
       <c r="E110" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="F110" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B111" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C111" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="D111" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="E111" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="F111" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B112" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C112" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="D112" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E112" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="F112" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B113" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C113" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D113" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="E113" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="F113" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B114" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C114" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="D114" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="E114" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="F114" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B115" t="s">
         <v>87</v>
       </c>
       <c r="C115" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="D115" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="E115" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="F115" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B116" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C116" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="D116" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="E116" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="F116" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B117" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C117" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D117" t="s">
-        <v>162</v>
+        <v>189</v>
       </c>
       <c r="E117" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="F117" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B118" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C118" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="D118" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E118" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="F118" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B119" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C119" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="D119" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="E119" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="F119" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="120" spans="1:6">
       <c r="A120">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B120" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C120" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="D120" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="E120" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="F120" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="121" spans="1:6">
       <c r="A121">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B121" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C121" t="s">
-        <v>149</v>
+        <v>110</v>
       </c>
       <c r="D121" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E121" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="F121" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122">
+        <v>131</v>
+      </c>
+      <c r="B122" t="s">
+        <v>92</v>
+      </c>
+      <c r="C122" t="s">
+        <v>153</v>
+      </c>
+      <c r="D122" t="s">
+        <v>158</v>
+      </c>
+      <c r="E122" t="s">
+        <v>291</v>
+      </c>
+      <c r="F122" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123">
+        <v>132</v>
+      </c>
+      <c r="B123" t="s">
+        <v>92</v>
+      </c>
+      <c r="C123" t="s">
+        <v>154</v>
+      </c>
+      <c r="D123" t="s">
+        <v>166</v>
+      </c>
+      <c r="E123" t="s">
+        <v>292</v>
+      </c>
+      <c r="F123" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124">
+        <v>134</v>
+      </c>
+      <c r="B124" t="s">
+        <v>93</v>
+      </c>
+      <c r="C124" t="s">
+        <v>155</v>
+      </c>
+      <c r="D124" t="s">
+        <v>190</v>
+      </c>
+      <c r="E124" t="s">
+        <v>293</v>
+      </c>
+      <c r="F124" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125">
+        <v>135</v>
+      </c>
+      <c r="B125" t="s">
+        <v>94</v>
+      </c>
+      <c r="C125" t="s">
+        <v>156</v>
+      </c>
+      <c r="D125" t="s">
+        <v>191</v>
+      </c>
+      <c r="E125" t="s">
+        <v>212</v>
+      </c>
+      <c r="F125" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126">
+        <v>137</v>
+      </c>
+      <c r="B126" t="s">
+        <v>95</v>
+      </c>
+      <c r="C126" t="s">
+        <v>140</v>
+      </c>
+      <c r="D126" t="s">
+        <v>182</v>
+      </c>
+      <c r="E126" t="s">
+        <v>212</v>
+      </c>
+      <c r="F126" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127">
         <v>138</v>
       </c>
-      <c r="B122" t="s">
-        <v>91</v>
-      </c>
-      <c r="C122" t="s">
-        <v>112</v>
-      </c>
-      <c r="D122" t="s">
-        <v>182</v>
-      </c>
-      <c r="E122" t="s">
-        <v>283</v>
-      </c>
-      <c r="F122" t="s">
-        <v>284</v>
+      <c r="B127" t="s">
+        <v>96</v>
+      </c>
+      <c r="C127" t="s">
+        <v>117</v>
+      </c>
+      <c r="D127" t="s">
+        <v>192</v>
+      </c>
+      <c r="E127" t="s">
+        <v>294</v>
+      </c>
+      <c r="F127" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: replace docstrings with type annotations in classes/methods
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Item</t>
   </si>
@@ -55,10 +55,13 @@
     <t>104910019</t>
   </si>
   <si>
-    <t>104910020</t>
+    <t>Não encontrado</t>
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>Pendente</t>
   </si>
 </sst>
 </file>
@@ -519,7 +522,7 @@
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: removed the responsibility of the RegistrationPDFService class to handle reports
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t>Item</t>
   </si>
@@ -34,37 +34,139 @@
     <t>PDF</t>
   </si>
   <si>
-    <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
-  </si>
-  <si>
-    <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 250ML</t>
-  </si>
-  <si>
-    <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 500ML</t>
-  </si>
-  <si>
-    <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
-  </si>
-  <si>
-    <t>1000ml</t>
-  </si>
-  <si>
-    <t>250ml</t>
-  </si>
-  <si>
-    <t>500ml</t>
-  </si>
-  <si>
-    <t>JP INDUSTRIA FARMACEUTICA S/A</t>
-  </si>
-  <si>
-    <t>104910019</t>
-  </si>
-  <si>
-    <t>104910020</t>
+    <t>HEPARINA SODICA SUBCUT 5000UI</t>
+  </si>
+  <si>
+    <t>PROMETAZINA 25MG, CLORIDRATO</t>
+  </si>
+  <si>
+    <t>HALOPERIDOL 5MG</t>
+  </si>
+  <si>
+    <t>CLORPROMAZINA 40MG/ML SOL ORAL</t>
+  </si>
+  <si>
+    <t>HALOPERIDOL 2MG/ML SOL ORAL</t>
+  </si>
+  <si>
+    <t>CLORPROMAZINA 25MG</t>
+  </si>
+  <si>
+    <t>CODEINA 30MG</t>
+  </si>
+  <si>
+    <t>IMIPRAMINA 25MG</t>
+  </si>
+  <si>
+    <t>RISPERIDONA 3MG</t>
+  </si>
+  <si>
+    <t>RISPERIDONA 1MG</t>
+  </si>
+  <si>
+    <t>LEVOMEPROMAZINA 4% GOTAS</t>
+  </si>
+  <si>
+    <t>LIDOCAINA 2% C/ VASO CONSTRITO</t>
+  </si>
+  <si>
+    <t>NITRATO DE CERIO +SULFADIAZINA</t>
+  </si>
+  <si>
+    <t>COLAGENASE+CLORAFENICOL POMADA 30g</t>
+  </si>
+  <si>
+    <t>5000ui</t>
+  </si>
+  <si>
+    <t>25mg</t>
+  </si>
+  <si>
+    <t>5mg</t>
+  </si>
+  <si>
+    <t>40mg/ml</t>
+  </si>
+  <si>
+    <t>2mg/ml</t>
+  </si>
+  <si>
+    <t>30mg</t>
+  </si>
+  <si>
+    <t>3mg</t>
+  </si>
+  <si>
+    <t>1mg</t>
+  </si>
+  <si>
+    <t>4%</t>
+  </si>
+  <si>
+    <t>2%</t>
+  </si>
+  <si>
+    <t>Concentração não encontrada</t>
+  </si>
+  <si>
+    <t>30g</t>
+  </si>
+  <si>
+    <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
+  </si>
+  <si>
+    <t>LABORATÓRIO TEUTO BRASILEIRO S/A</t>
+  </si>
+  <si>
+    <t>CELLERA FARMACÊUTICA S.A.</t>
+  </si>
+  <si>
+    <t>SANOFI MEDLEY FARMACÊUTICA LTDA</t>
+  </si>
+  <si>
+    <t>VITAMEDIC INDUSTRIA FARMACEUTICA LTDA</t>
+  </si>
+  <si>
+    <t>102980371</t>
+  </si>
+  <si>
+    <t>103700321</t>
+  </si>
+  <si>
+    <t>112360011</t>
+  </si>
+  <si>
+    <t>Último registro encontrado: 183260385</t>
+  </si>
+  <si>
+    <t>183260385</t>
+  </si>
+  <si>
+    <t>102980199</t>
+  </si>
+  <si>
+    <t>102980023</t>
+  </si>
+  <si>
+    <t>103920197</t>
+  </si>
+  <si>
+    <t>Último registro encontrado: 183260316</t>
+  </si>
+  <si>
+    <t>102980249</t>
+  </si>
+  <si>
+    <t>Último registro encontrado: 102980560</t>
+  </si>
+  <si>
+    <t>102980431</t>
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>Pendente</t>
   </si>
 </sst>
 </file>
@@ -422,7 +524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,82 +552,282 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
         <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
migrate project from venv to poetry
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -1,96 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Descrição</t>
-  </si>
-  <si>
-    <t>Concentração_Encontrada</t>
-  </si>
-  <si>
-    <t>Marca</t>
-  </si>
-  <si>
-    <t>Registro</t>
-  </si>
-  <si>
-    <t>PDF</t>
-  </si>
-  <si>
-    <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
-  </si>
-  <si>
-    <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 250ML</t>
-  </si>
-  <si>
-    <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 500ML</t>
-  </si>
-  <si>
-    <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
-  </si>
-  <si>
-    <t>1000ml</t>
-  </si>
-  <si>
-    <t>250ml</t>
-  </si>
-  <si>
-    <t>500ml</t>
-  </si>
-  <si>
-    <t>JP INDUSTRIA FARMACEUTICA S/A</t>
-  </si>
-  <si>
-    <t>104910019</t>
-  </si>
-  <si>
-    <t>104910020</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -105,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -421,114 +420,172 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Descrição</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Concentração_Encontrada</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Marca</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Registro</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>PDF</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
+    <row r="2">
+      <c r="A2" t="n">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1000ml</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Último registro encontrado: 104910019</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
+    <row r="3">
+      <c r="A3" t="n">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 250ML</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>250ml</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Último registro encontrado: 104910019</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
+    <row r="4">
+      <c r="A4" t="n">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 500ML</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>500ml</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Último registro encontrado: 104910019</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
+    <row r="5">
+      <c r="A5" t="n">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1000ml</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>104910020</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: adjusted XPath after website structure change by ANVISA
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -486,12 +486,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Último registro encontrado: 104910019</t>
+          <t>104910019</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Pendente</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -516,12 +516,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Último registro encontrado: 104910019</t>
+          <t>104910019</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Pendente</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -546,12 +546,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Último registro encontrado: 104910019</t>
+          <t>104910019</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Pendente</t>
+          <t>OK</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: fixed some interface bugs
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,26 +467,26 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
+          <t>HEPARINA SODICA SUBCUT 5000UI</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1000ml</t>
+          <t>5000ui</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
+          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>104910019</t>
+          <t>102980371</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -497,26 +497,26 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 250ML</t>
+          <t>PROMETAZINA 25MG, CLORIDRATO</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>250ml</t>
+          <t>25mg</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
+          <t>LABORATÓRIO TEUTO BRASILEIRO S/A</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>104910019</t>
+          <t>103700321</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -527,26 +527,26 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 500ML</t>
+          <t>HALOPERIDOL 5MG</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>500ml</t>
+          <t>5mg</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
+          <t>CELLERA FARMACÊUTICA S.A.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>104910019</t>
+          <t>112360011</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -557,29 +557,329 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CLORPROMAZINA 40MG/ML SOL ORAL</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>40mg/ml</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>SANOFI MEDLEY FARMACÊUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Último registro encontrado: 183260385</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>HALOPERIDOL 2MG/ML SOL ORAL</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2mg/ml</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>CELLERA FARMACÊUTICA S.A.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>112360011</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>8</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CLORPROMAZINA 25MG</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>25mg</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>SANOFI MEDLEY FARMACÊUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>183260385</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>9</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1000ml</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>104910020</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CODEINA 30MG</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>30mg</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>102980199</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>10</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>IMIPRAMINA 25MG</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>25mg</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>102980023</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>11</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>RISPERIDONA 3MG</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>3mg</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>VITAMEDIC INDUSTRIA FARMACEUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>103920197</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>13</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>RISPERIDONA 1MG</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1mg</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>VITAMEDIC INDUSTRIA FARMACEUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>103920197</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>14</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>LEVOMEPROMAZINA 4% GOTAS</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>4%</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>SANOFI MEDLEY FARMACÊUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Último registro encontrado: 183260316</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>16</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>LIDOCAINA 2% C/ VASO CONSTRITO</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2%</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>102980249</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>17</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>NITRATO DE CERIO +SULFADIAZINA</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Concentração não encontrada</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Último registro encontrado: 102980560</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>18</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>COLAGENASE+CLORAFENICOL POMADA 30g</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>30g</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>102980431</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
         <is>
           <t>OK</t>
         </is>

</xml_diff>

<commit_message>
refactor: improved report information
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,17 +446,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Concentração_Encontrada</t>
+          <t>Marca</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Marca</t>
+          <t>Registro</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Registro</t>
+          <t>Apresentação</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -467,26 +467,26 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
+          <t>HEPARINA SODICA SUBCUT 5000UI</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1000ml</t>
+          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
+          <t>102980371</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>104910019</t>
+          <t>5000 UI/ML SOL INJ CX 25 FA VD INC X 5 ML ATIVA</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -497,26 +497,26 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 250ML</t>
+          <t>PROMETAZINA 25MG, CLORIDRATO</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>250ml</t>
+          <t>LABORATÓRIO TEUTO BRASILEIRO S/A</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
+          <t>103700321</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>104910019</t>
+          <t>25 MG COM REV BL AL PLAS INC X 200 (EMB. HOSP.) ATIVA</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -527,26 +527,26 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 500ML</t>
+          <t>HALOPERIDOL 5MG</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>500ml</t>
+          <t>CELLERA FARMACÊUTICA S.A.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
+          <t>112360011</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>104910019</t>
+          <t>5 MG COM CT BL AL PLAS TRANS X 20 ATIVA</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -557,29 +557,329 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CLORPROMAZINA 40MG/ML SOL ORAL</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SANOFI MEDLEY FARMACÊUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Último registro encontrado: 183260385</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>HALOPERIDOL 2MG/ML SOL ORAL</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CELLERA FARMACÊUTICA S.A.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>112360011</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2 MG/ML SOL GOT OR CT FR GOT PLAS OPC X 30 ML ATIVA</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>8</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CLORPROMAZINA 25MG</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SANOFI MEDLEY FARMACÊUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>183260385</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>25 MG COM REV CT BL AL PLAS OPC X 20 ATIVA</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>9</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1000ml</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>104910020</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CODEINA 30MG</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>102980199</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>30 MG COM CT BL AL PLAS TRANS X 30 ATIVA</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>10</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>IMIPRAMINA 25MG</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>102980023</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>25 MG COM REV CX 20 ENV AL POLIET X 10 (EMB HOSP) CANCELADA OU CADUCA</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>11</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>RISPERIDONA 3MG</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>VITAMEDIC INDUSTRIA FARMACEUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>103920197</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>3 MG COM REV CT BL AL PLAS TRANS X 10 ATIVA</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>13</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>RISPERIDONA 1MG</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>VITAMEDIC INDUSTRIA FARMACEUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>103920197</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1 MG COM REV CT BL AL PLAS TRANS X 10 ATIVA</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>14</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>LEVOMEPROMAZINA 4% GOTAS</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>SANOFI MEDLEY FARMACÊUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Último registro encontrado: 183260316</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>16</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>LIDOCAINA 2% C/ VASO CONSTRITO</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>102980249</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2% GEL TOP CT BG AL X 30 G + APLIC ATIVA</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>17</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>NITRATO DE CERIO +SULFADIAZINA</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Último registro encontrado: 102980560</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Não encontrado</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>18</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>COLAGENASE+CLORAFENICOL POMADA 30g</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>102980431</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>0,6 U/G POM DERM CT 01 BG AL X 30 G + ESP PLAS ATIVA</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
         <is>
           <t>OK</t>
         </is>

</xml_diff>

<commit_message>
refactor: improved filter to search only active medications + optimized login system +  minor bug fixes
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -486,7 +486,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>5000 UI/ML SOL INJ CX 25 FA VD INC X 5 ML ATIVA</t>
+          <t>5000 UI/ML SOL INJ IV CX 1 EST PLAS X 1 FA VD TRANS X 5 ML (EMB HOSP) Ativo</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>25 MG COM REV BL AL PLAS INC X 200 (EMB. HOSP.) ATIVA</t>
+          <t>25 MG COM REV BL AL PLAS INC X 200 (EMB. HOSP.) Ativo</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -546,7 +546,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>5 MG COM CT BL AL PLAS TRANS X 20 ATIVA</t>
+          <t>5 MG COM CT BL AL PLAS TRANS X 20 Ativo</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2 MG/ML SOL GOT OR CT FR GOT PLAS OPC X 30 ML ATIVA</t>
+          <t>2 MG/ML SOL GOT OR CT FR GOT PLAS OPC X 30 ML Ativo</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -636,7 +636,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>25 MG COM REV CT BL AL PLAS OPC X 20 ATIVA</t>
+          <t>25 MG COM REV CT BL AL PLAS OPC X 20 Ativo</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -666,7 +666,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>30 MG COM CT BL AL PLAS TRANS X 30 ATIVA</t>
+          <t>30 MG COM CT BL AL PLAS PVC/PVDC TRANS X 30 Ativo</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>25 MG COM REV CX 20 ENV AL POLIET X 10 (EMB HOSP) CANCELADA OU CADUCA</t>
+          <t>25 MG COM REV CT BL AL PLAS PVDC TRANS X 20 Ativo</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -726,7 +726,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>3 MG COM REV CT BL AL PLAS TRANS X 10 ATIVA</t>
+          <t>3 MG COM REV CT BL AL PLAS TRANS X 10 Ativo</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -756,7 +756,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1 MG COM REV CT BL AL PLAS TRANS X 10 ATIVA</t>
+          <t>1 MG COM REV CT BL AL PLAS TRANS X 10 Ativo</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -811,17 +811,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>102980249</t>
+          <t>Último registro encontrado: 102980249</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2% GEL TOP CT BG AL X 30 G + APLIC ATIVA</t>
+          <t>Não encontrado</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>Pendente</t>
         </is>
       </c>
     </row>
@@ -876,7 +876,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0,6 U/G POM DERM CT 01 BG AL X 30 G + ESP PLAS ATIVA</t>
+          <t>1,2 U/G POM DERM CT 10 BG AL X 30 G + ESP PLAS Ativo</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">

</xml_diff>

<commit_message>
feat: visual feedback of app progression added
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,26 +467,26 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>HEPARINA SODICA SUBCUT 5000UI</t>
+          <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
+          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>102980371</t>
+          <t>104910019</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>5000 UI/ML SOL INJ IV CX 1 EST PLAS X 1 FA VD TRANS X 5 ML (EMB HOSP) Ativo</t>
+          <t>(9 + 50) MG/ML SOL INJ IV CX 10 BOLS PLAS PVC TRANS SIST FECH X 1000 ML  Ativo</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -497,26 +497,26 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>PROMETAZINA 25MG, CLORIDRATO</t>
+          <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 250ML</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>LABORATÓRIO TEUTO BRASILEIRO S/A</t>
+          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>103700321</t>
+          <t>104910019</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>25 MG COM REV BL AL PLAS INC X 200 (EMB. HOSP.) Ativo</t>
+          <t>(9 + 50) MG/ML SOL INJ IV CX 35 BOLS PLAS PVC TRANS SIST FECH X 250 ML Ativo</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -527,26 +527,26 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>HALOPERIDOL 5MG</t>
+          <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 500ML</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CELLERA FARMACÊUTICA S.A.</t>
+          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>112360011</t>
+          <t>104910019</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>5 MG COM CT BL AL PLAS TRANS X 20 Ativo</t>
+          <t>(9 + 50) MG/ML SOL INJ IV CX 20 BOLS PLAS PVC TRANS SIST FECH X 500 ML Ativo</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -557,329 +557,29 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CLORPROMAZINA 40MG/ML SOL ORAL</t>
+          <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SANOFI MEDLEY FARMACÊUTICA LTDA</t>
+          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Último registro encontrado: 183260385</t>
+          <t>104910020</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Não encontrado</t>
+          <t>50 MG/ML SOL INJ IV CX 10 BOLS PLAS SIST FECH X 1000 ML Ativo</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
-        <is>
-          <t>Pendente</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>7</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>HALOPERIDOL 2MG/ML SOL ORAL</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>CELLERA FARMACÊUTICA S.A.</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>112360011</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2 MG/ML SOL GOT OR CT FR GOT PLAS OPC X 30 ML Ativo</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>8</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>CLORPROMAZINA 25MG</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>SANOFI MEDLEY FARMACÊUTICA LTDA</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>183260385</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>25 MG COM REV CT BL AL PLAS OPC X 20 Ativo</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>9</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>CODEINA 30MG</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>102980199</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>30 MG COM CT BL AL PLAS PVC/PVDC TRANS X 30 Ativo</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>10</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>IMIPRAMINA 25MG</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>102980023</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>25 MG COM REV CT BL AL PLAS PVDC TRANS X 20 Ativo</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>11</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>RISPERIDONA 3MG</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>VITAMEDIC INDUSTRIA FARMACEUTICA LTDA</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>103920197</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>3 MG COM REV CT BL AL PLAS TRANS X 10 Ativo</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>13</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>RISPERIDONA 1MG</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>VITAMEDIC INDUSTRIA FARMACEUTICA LTDA</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>103920197</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>1 MG COM REV CT BL AL PLAS TRANS X 10 Ativo</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>14</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>LEVOMEPROMAZINA 4% GOTAS</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>SANOFI MEDLEY FARMACÊUTICA LTDA</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Último registro encontrado: 183260316</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Não encontrado</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Pendente</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>16</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>LIDOCAINA 2% C/ VASO CONSTRITO</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Último registro encontrado: 102980249</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Não encontrado</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Pendente</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>17</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>NITRATO DE CERIO +SULFADIAZINA</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Último registro encontrado: 102980560</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Não encontrado</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Pendente</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>18</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>COLAGENASE+CLORAFENICOL POMADA 30g</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>CRISTÁLIA PRODUTOS QUÍMICOS FARMACÊUTICOS LTDA</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>102980431</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>1,2 U/G POM DERM CT 10 BG AL X 30 G + ESP PLAS Ativo</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
         <is>
           <t>OK</t>
         </is>

</xml_diff>

<commit_message>
feat: it is now possible to search individually for medication registers
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,120 +466,32 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>6</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
+          <t>Aciclovir 200mg</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
+          <t>CIMED INDUSTRIA S.A</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>104910019</t>
+          <t>143810181</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>(9 + 50) MG/ML SOL INJ IV CX 10 BOLS PLAS PVC TRANS SIST FECH X 1000 ML  Ativo</t>
+          <t>200 MG COM CT BL AL PLAS TRANS X 10  Ativo</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>7</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 250ML</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>104910019</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>(9 + 50) MG/ML SOL INJ IV CX 35 BOLS PLAS PVC TRANS SIST FECH X 250 ML Ativo</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>8</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>SORO GLICOFISIOLÓGICO, GLICOSE À 5% EM CLORETO DE SÓDIO À 0,9%; BOLSA SISTEMA FECHADO, FRASCO COM 500ML</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>104910019</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>(9 + 50) MG/ML SOL INJ IV CX 20 BOLS PLAS PVC TRANS SIST FECH X 500 ML Ativo</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>9</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>104910020</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>50 MG/ML SOL INJ IV CX 10 BOLS PLAS SIST FECH X 1000 ML Ativo</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
         <is>
           <t>OK</t>
         </is>

</xml_diff>

<commit_message>
feat: error handling for incorrect column names with visual feedback for users added
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -466,29 +466,27 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>9</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Aciclovir 200mg</t>
+          <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CIMED INDUSTRIA S.A</t>
+          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>143810181</t>
+          <t>104910020</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>200 MG COM CT BL AL PLAS TRANS X 10  Ativo</t>
+          <t>50 MG/ML SOL INJ IV CX 10 BOLS PLAS SIST FECH X 1000 ML Ativo</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">

</xml_diff>

<commit_message>
fix: clear file path when canceling selection
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -466,32 +466,34 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>9</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ITEM</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
+          <t>DESCRIÇÃO</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
+          <t>MARCA</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>104910020</t>
+          <t>Não encontrado</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>50 MG/ML SOL INJ IV CX 10 BOLS PLAS SIST FECH X 1000 ML Ativo</t>
+          <t>Não encontrado</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>Pendente</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: logging system reformulated
</commit_message>
<xml_diff>
--- a/relatorio_registros.xlsx
+++ b/relatorio_registros.xlsx
@@ -466,34 +466,32 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ITEM</t>
-        </is>
+      <c r="A2" t="n">
+        <v>9</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DESCRIÇÃO</t>
+          <t>SORO GLICOSADO 5%, BOLSA SISTEMA FECHADO, FRASCO COM 1000ML</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MARCA</t>
+          <t>JP INDUSTRIA FARMACEUTICA S/A</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Não encontrado</t>
+          <t>104910020</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Não encontrado</t>
+          <t>50 MG/ML SOL INJ IV CX 10 BOLS PLAS SIST FECH X 1000 ML Ativo</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Pendente</t>
+          <t>OK</t>
         </is>
       </c>
     </row>

</xml_diff>